<commit_message>
Commit Screen Design & Quality Report + update Dữ liệu Demo
</commit_message>
<xml_diff>
--- a/WIP/Users/HaiCM/Dữ liệu demo/Dữ liệu demo.xlsx
+++ b/WIP/Users/HaiCM/Dữ liệu demo/Dữ liệu demo.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GAULUOI\Desktop\Dữ liệu demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sách" sheetId="1" r:id="rId1"/>
     <sheet name="Nhóm" sheetId="2" r:id="rId2"/>
+    <sheet name="Tác giả &amp; NXB &amp; Category" sheetId="3" r:id="rId3"/>
+    <sheet name="Post" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="240">
   <si>
     <t>STT</t>
   </si>
@@ -284,9 +287,6 @@
   </si>
   <si>
     <t> 05/2014</t>
-  </si>
-  <si>
-    <t>Tâm ký</t>
   </si>
   <si>
     <t>Chúng Ta Rồi Sẽ Ổn Thôi</t>
@@ -676,6 +676,180 @@
 Bạn muốn chốt sale nhanh?
 Đến vs Kỹ năng của một Saler bạn sẽ khám phá những kỹ năng đưa bạn trở thành 1 Saler thành công</t>
   </si>
+  <si>
+    <t>Tên tác giả</t>
+  </si>
+  <si>
+    <t>Gào</t>
+  </si>
+  <si>
+    <t>Năm sinh-Năm mất</t>
+  </si>
+  <si>
+    <t>1955-?</t>
+  </si>
+  <si>
+    <t>1802-1885</t>
+  </si>
+  <si>
+    <t>1988-?</t>
+  </si>
+  <si>
+    <t>1952-?</t>
+  </si>
+  <si>
+    <t>1904-1936</t>
+  </si>
+  <si>
+    <t>1949-?</t>
+  </si>
+  <si>
+    <t>1958-?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1962-?</t>
+  </si>
+  <si>
+    <t>1974-?</t>
+  </si>
+  <si>
+    <t>1965-?</t>
+  </si>
+  <si>
+    <t>Tên NXB</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>Điện thoại</t>
+  </si>
+  <si>
+    <t>46 Trần Hưng Đạo, Hàng Bài, Hoàn Kiếm, Hà Nội</t>
+  </si>
+  <si>
+    <t>04 3825 3841</t>
+  </si>
+  <si>
+    <t>55 Quang Trung, Hà Nội</t>
+  </si>
+  <si>
+    <t>04 3943 4730</t>
+  </si>
+  <si>
+    <t>Số 18 Nguyễn Trường Tộ, Trúc Bạch, Ba Đình, Hà Nội</t>
+  </si>
+  <si>
+    <t>04 3716 1518</t>
+  </si>
+  <si>
+    <t>39 Hàng Chuối, Quận Hai Bà Trưng, Thành Phố Hà Nội</t>
+  </si>
+  <si>
+    <t>04 3971 0717</t>
+  </si>
+  <si>
+    <t>08 3931 6289</t>
+  </si>
+  <si>
+    <t>65 Nguyễn Du, Hai Bà Trưng, Hà Nội</t>
+  </si>
+  <si>
+    <t>04 3822 1406</t>
+  </si>
+  <si>
+    <t>62 Nguyễn Thị Minh Khai, Đa Kao, Quận 1, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>08 3822 5340</t>
+  </si>
+  <si>
+    <t>Số 36 Ngõ Hòa Bình 4, phố Minh Khai, Hai Bà Trưng, Hà Nội</t>
+  </si>
+  <si>
+    <t>04 3624 6913</t>
+  </si>
+  <si>
+    <t>26 Lý Thường Kiệt, Hoàn Kiếm, Hà Nội</t>
+  </si>
+  <si>
+    <t>75 Arlington Street, Suite 300 in Boston, Mass</t>
+  </si>
+  <si>
+    <t>617-848-7500</t>
+  </si>
+  <si>
+    <t>NHÀ XUẤT BẢN</t>
+  </si>
+  <si>
+    <t>TÁC GIẢ</t>
+  </si>
+  <si>
+    <t>CATEGORY</t>
+  </si>
+  <si>
+    <t>Tình cảm</t>
+  </si>
+  <si>
+    <t>Truyện thiếu nhi</t>
+  </si>
+  <si>
+    <t>Giả tưởng</t>
+  </si>
+  <si>
+    <t>Phiêu lưu</t>
+  </si>
+  <si>
+    <t>Kinh tế</t>
+  </si>
+  <si>
+    <t>Tâm lý</t>
+  </si>
+  <si>
+    <t>Khoa học - Tự nhiên</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Nội dung post</t>
+  </si>
+  <si>
+    <t>Trời ơi tui thích thầy Snape dữ ah. Đúng chuẩn cold man từ đầu đến cuối luôngg</t>
+  </si>
+  <si>
+    <t>Nơi post</t>
+  </si>
+  <si>
+    <t>Cá nhân</t>
+  </si>
+  <si>
+    <t>Group: "IT's Dev"</t>
+  </si>
+  <si>
+    <t>Cả nhà ơi hình như sắp tới có 1 khóa học Tôi tài giỏi của Adam Khoo ở HCM đấy có bạn nào có thông tin chi tiết không?</t>
+  </si>
+  <si>
+    <t>Group: "Nguyễn Nhật Ánh - Nhà văn của tuổi thơ"</t>
+  </si>
+  <si>
+    <t>Có ai biết nhà sách nào bán cuốn Tư duy nhanh và chậm không nhỉ?</t>
+  </si>
+  <si>
+    <t>Group: "Tâm lí chiến trong kinh doanh"</t>
+  </si>
+  <si>
+    <t>Mình có nghe nói cuốn sách The Clean Coder rất hay. Có sempai nào đã từng đọc qua review cho mình với?</t>
+  </si>
+  <si>
+    <t>Group: "Frontend Developers"</t>
+  </si>
+  <si>
+    <t>JavaScript: The Good Parts là một tựa sách kinh điển ra đời vào năm 2008, được nhiều lập trình viên Javascript giỏi khuyến cáo là nên đọc khi bạn bắt đầu với Javascript, thật ra thì tới tận 2014 tôi mới đọc nó. Tác giả Douglas Crockford, cũng là một người khá quen thuộc trong cộng đồng Javascript và cũng là một thành viên trong hội đồng ECMAScript.
+Mặc dù ra đời khá lâu và đến giờ phút này có thể coi là lỗi thời vì quyển sách chỉ bao gồm các đặc điểm kỹ thuật của ES3 thì quyển sách này vẫn cực kì giá trị cho đến tận hôm nay vì những bài học mà nó mang lại.
+Đây là một quyển sách dễ đọc, những thứ cơ bản nhất của Javascript được tóm gọn trong chỉ khoảng 100 trang. Cực kì phù hợp để bạn có thể nắm bắt hết những phần cơ bản của Javascript trong một vài ngày, lưu ý là chỉ những phần cơ bản thôi nhé, những phần phức tạp như inheritance, modify built-in objects… thì cũng ngốn kha khá thời gian của bạn đấy. Và dù cho thế, thì nó vẫn là một quyển sách cực kì dễ đọc.
+Xem thêm tại: https://codeaholicguy.com/2016/06/21/chuyen-xua-cu-ai-chua-doc-javascript-the-good-parts/</t>
+  </si>
 </sst>
 </file>
 
@@ -684,7 +858,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -720,8 +894,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -746,8 +936,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -831,11 +1033,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -915,14 +1141,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="30">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -2753,16 +3054,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G12" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="A2:G12"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="STT" dataDxfId="6"/>
-    <tableColumn id="2" name="Tên nhóm" dataDxfId="5"/>
-    <tableColumn id="3" name="Tag sách" dataDxfId="4"/>
-    <tableColumn id="4" name="Tag tác giả" dataDxfId="3"/>
-    <tableColumn id="5" name="Kiểu nhóm" dataDxfId="2"/>
-    <tableColumn id="6" name="Miêu tả" dataDxfId="1"/>
-    <tableColumn id="7" name="Note" dataDxfId="0"/>
+    <tableColumn id="1" name="STT" dataDxfId="24"/>
+    <tableColumn id="2" name="Tên nhóm" dataDxfId="23"/>
+    <tableColumn id="3" name="Tag sách" dataDxfId="22"/>
+    <tableColumn id="4" name="Tag tác giả" dataDxfId="21"/>
+    <tableColumn id="5" name="Kiểu nhóm" dataDxfId="20"/>
+    <tableColumn id="6" name="Miêu tả" dataDxfId="19"/>
+    <tableColumn id="7" name="Note" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:D12" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="B2:D12"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="STT" dataDxfId="15"/>
+    <tableColumn id="2" name="Tên tác giả" dataDxfId="14"/>
+    <tableColumn id="3" name="Năm sinh-Năm mất" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="F2:I12" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="F2:I12"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="STT" dataDxfId="10"/>
+    <tableColumn id="2" name="Tên NXB" dataDxfId="9"/>
+    <tableColumn id="3" name="Địa chỉ" dataDxfId="8"/>
+    <tableColumn id="4" name="Điện thoại" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:E13" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E13"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="STT" dataDxfId="4"/>
+    <tableColumn id="2" name="Nội dung post" dataDxfId="3"/>
+    <tableColumn id="3" name="Nơi post" dataDxfId="2"/>
+    <tableColumn id="4" name="Tag sách" dataDxfId="1"/>
+    <tableColumn id="5" name="Tag tác giả" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3069,8 +3409,8 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3087,17 +3427,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3149,7 +3489,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I3" s="5"/>
     </row>
@@ -3174,7 +3514,7 @@
         <v>32</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I4" s="8"/>
     </row>
@@ -3224,7 +3564,7 @@
         <v>22</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I6" s="8"/>
     </row>
@@ -3249,7 +3589,7 @@
         <v>26</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I7" s="5"/>
     </row>
@@ -3274,7 +3614,7 @@
         <v>31</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I8" s="8"/>
     </row>
@@ -3324,7 +3664,7 @@
         <v>45</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I10" s="8"/>
     </row>
@@ -3349,7 +3689,7 @@
         <v>44</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I11" s="5"/>
     </row>
@@ -3449,7 +3789,7 @@
         <v>57</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I15" s="5"/>
     </row>
@@ -3571,10 +3911,10 @@
         <v>80</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>81</v>
+        <v>225</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I20" s="8"/>
     </row>
@@ -3584,22 +3924,22 @@
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="H21" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I21" s="5"/>
     </row>
@@ -3609,7 +3949,7 @@
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>51</v>
@@ -3618,13 +3958,13 @@
         <v>35</v>
       </c>
       <c r="F22" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="G22" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="H22" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I22" s="8"/>
     </row>
@@ -3634,20 +3974,20 @@
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I23" s="5"/>
     </row>
@@ -3657,22 +3997,22 @@
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D24" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="F24" s="12">
         <v>40664</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I24" s="8"/>
     </row>
@@ -3682,22 +4022,22 @@
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="G25" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>102</v>
       </c>
       <c r="I25" s="5"/>
     </row>
@@ -3707,22 +4047,22 @@
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="E26" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F26" s="12">
         <v>42407</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I26" s="8"/>
     </row>
@@ -3732,22 +4072,22 @@
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>109</v>
       </c>
       <c r="F27" s="13">
         <v>39569</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I27" s="5"/>
     </row>
@@ -3757,22 +4097,22 @@
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>113</v>
       </c>
       <c r="F28" s="12">
         <v>40686</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I28" s="8"/>
     </row>
@@ -3782,22 +4122,22 @@
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="F29" s="13">
         <v>38157</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I29" s="5"/>
     </row>
@@ -3807,22 +4147,22 @@
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>120</v>
-      </c>
       <c r="E30" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F30" s="12">
         <v>34923</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I30" s="8"/>
     </row>
@@ -3832,22 +4172,22 @@
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>125</v>
-      </c>
       <c r="E31" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F31" s="13">
         <v>36192</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I31" s="5"/>
     </row>
@@ -3857,22 +4197,22 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>129</v>
-      </c>
       <c r="E32" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F32" s="12">
         <v>41642</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I32" s="8"/>
     </row>
@@ -3882,22 +4222,22 @@
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D33" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="F33" s="13">
         <v>35258</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I33" s="5"/>
     </row>
@@ -3907,22 +4247,22 @@
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>136</v>
       </c>
       <c r="F34" s="12">
         <v>37518</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I34" s="8"/>
     </row>
@@ -3932,22 +4272,22 @@
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F35" s="13">
         <v>39209</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I35" s="5"/>
     </row>
@@ -4056,9 +4396,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4073,31 +4413,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>153</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="A1" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="D2" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="E2" s="19" t="s">
         <v>156</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>157</v>
       </c>
       <c r="F2" s="25" t="s">
         <v>6</v>
@@ -4111,17 +4451,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>158</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>159</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>160</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>161</v>
       </c>
       <c r="G3" s="23"/>
     </row>
@@ -4130,17 +4470,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>164</v>
       </c>
       <c r="G4" s="23"/>
     </row>
@@ -4149,17 +4489,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>165</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>166</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G5" s="23"/>
     </row>
@@ -4168,17 +4508,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G6" s="23"/>
     </row>
@@ -4187,17 +4527,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>171</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>172</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G7" s="23"/>
     </row>
@@ -4206,14 +4546,14 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>174</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>175</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="23"/>
@@ -4223,17 +4563,17 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22" t="s">
         <v>29</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G9" s="23"/>
     </row>
@@ -4242,17 +4582,17 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>178</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>179</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G10" s="23"/>
     </row>
@@ -4261,14 +4601,14 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="23"/>
@@ -4278,17 +4618,17 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>59</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G12" s="23"/>
     </row>
@@ -4310,4 +4650,550 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="28" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" style="24" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" style="24" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" style="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="34" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="F1" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="K1" s="34" t="s">
+        <v>219</v>
+      </c>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="M2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="30" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="24">
+        <v>1</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="F3" s="24">
+        <v>1</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="K3" s="31">
+        <v>1</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="M3" s="31">
+        <v>11</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="24">
+        <v>2</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="F4" s="24">
+        <v>2</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="K4" s="31">
+        <v>2</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="31">
+        <v>12</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="24">
+        <v>3</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="F5" s="24">
+        <v>3</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="K5" s="31">
+        <v>3</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="31">
+        <v>13</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="24">
+        <v>4</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="24">
+        <v>4</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="K6" s="31">
+        <v>4</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="31">
+        <v>14</v>
+      </c>
+      <c r="N6" s="24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="24">
+        <v>5</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="F7" s="24">
+        <v>5</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="K7" s="31">
+        <v>5</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="24">
+        <v>6</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="F8" s="24">
+        <v>6</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="K8" s="31">
+        <v>6</v>
+      </c>
+      <c r="L8" s="24" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="24">
+        <v>7</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="F9" s="24">
+        <v>7</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="K9" s="31">
+        <v>7</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="24">
+        <v>8</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="F10" s="24">
+        <v>8</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="I10" s="28">
+        <v>4.3971907300000002</v>
+      </c>
+      <c r="K10" s="31">
+        <v>8</v>
+      </c>
+      <c r="L10" s="24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="24">
+        <v>9</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="F11" s="24">
+        <v>9</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="K11" s="31">
+        <v>9</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="24">
+        <v>10</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F12" s="24">
+        <v>10</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="K12" s="31">
+        <v>10</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="101.140625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="16" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11" style="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="24">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>2</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>3</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>6</v>
+      </c>
+      <c r="B7" s="32"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
+        <v>7</v>
+      </c>
+      <c r="B8" s="32"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>8</v>
+      </c>
+      <c r="B9" s="32"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
+        <v>9</v>
+      </c>
+      <c r="B10" s="32"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>10</v>
+      </c>
+      <c r="B11" s="32"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="24">
+        <v>11</v>
+      </c>
+      <c r="B12" s="32"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>